<commit_message>
Fixing writeups for coverage and population
</commit_message>
<xml_diff>
--- a/data/marikina_evac_centers.xlsx
+++ b/data/marikina_evac_centers.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianesamson/Projects/riesgo-vis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{259E99B1-84E3-E542-B635-76BC154A55EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEF6424-C303-A143-9701-45FA88BB2E28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="marikina_evac_centers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="46">
   <si>
     <t>osm_id</t>
   </si>
@@ -160,12 +160,18 @@
   </si>
   <si>
     <t>pop_coverage</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>% growth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1000,20 +1006,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="10" max="11" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1044,8 +1050,14 @@
       <c r="J1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5168988</v>
       </c>
@@ -1077,8 +1089,20 @@
       <c r="J2">
         <v>11444.65</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <f>J2/I2</f>
+        <v>3.7077996087657721</v>
+      </c>
+      <c r="L2">
+        <f>J2-I2</f>
+        <v>8358.0079999999998</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(L2:L29)</f>
+        <v>10416.448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5168990</v>
       </c>
@@ -1110,8 +1134,20 @@
       <c r="J3">
         <v>9276.84</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <f t="shared" ref="K3:K29" si="1">J3/I3</f>
+        <v>4.122922725753579</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L29" si="2">J3-I3</f>
+        <v>7026.7759999999998</v>
+      </c>
+      <c r="M3">
+        <f>MEDIAN(L2:L29)</f>
+        <v>10033.790000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5235831</v>
       </c>
@@ -1143,8 +1179,16 @@
       <c r="J4">
         <v>13175.09</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>4.4714555090670656</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>10228.601999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5644348</v>
       </c>
@@ -1176,8 +1220,16 @@
       <c r="J5">
         <v>12247.09</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>6.6457262981509091</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>10404.237999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5708235</v>
       </c>
@@ -1209,8 +1261,16 @@
       <c r="J6">
         <v>12925.11</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>5.1013472178258699</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>10391.444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6494760</v>
       </c>
@@ -1242,8 +1302,16 @@
       <c r="J7">
         <v>7487.83</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>2.090850756554441</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>3906.5940000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>25055845</v>
       </c>
@@ -1275,8 +1343,16 @@
       <c r="J8">
         <v>9576.7800000000007</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2.6321405013192614</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>5938.380000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>41741656</v>
       </c>
@@ -1308,8 +1384,16 @@
       <c r="J9">
         <v>11079.37</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>17.402990091669338</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>10442.734</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>46331655</v>
       </c>
@@ -1341,8 +1425,16 @@
       <c r="J10">
         <v>10629.44</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>7.4868919661346442</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>9209.7000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>46507461</v>
       </c>
@@ -1374,8 +1466,16 @@
       <c r="J11">
         <v>7163.72</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>6.3195985786522613</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>6030.1480000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>48209843</v>
       </c>
@@ -1407,8 +1507,16 @@
       <c r="J12">
         <v>9267.61</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>4.8635238206193119</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>7362.0760000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>48210073</v>
       </c>
@@ -1440,8 +1548,16 @@
       <c r="J13">
         <v>17706.919999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>7.4515606391529579</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>15330.649999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>50982403</v>
       </c>
@@ -1473,8 +1589,16 @@
       <c r="J14">
         <v>21574.85</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>8.3841763164705601</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>19001.567999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>50982404</v>
       </c>
@@ -1506,8 +1630,16 @@
       <c r="J15">
         <v>14986.52</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>7.9048747321793087</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>13090.662</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>93199293</v>
       </c>
@@ -1539,8 +1671,16 @@
       <c r="J16">
         <v>10380.870000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>71.256074792015596</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>10235.186000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>93320662</v>
       </c>
@@ -1572,8 +1712,16 @@
       <c r="J17">
         <v>7529.73</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>20.654975476480463</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>7165.1819999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>93320668</v>
       </c>
@@ -1605,8 +1753,16 @@
       <c r="J18">
         <v>7762</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>19.710112542152523</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>7368.192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>106995109</v>
       </c>
@@ -1635,8 +1791,16 @@
       <c r="J19">
         <v>12403.98</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>88.095197511398993</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>12263.178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>116914599</v>
       </c>
@@ -1665,8 +1829,16 @@
       <c r="J20">
         <v>20766.740000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>167.85815900934398</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>20643.024000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>116914602</v>
       </c>
@@ -1695,8 +1867,16 @@
       <c r="J21">
         <v>18983.150000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>127.05067798198294</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>18833.736000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>256400347</v>
       </c>
@@ -1725,8 +1905,16 @@
       <c r="J22">
         <v>10108.200000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>37.545965782885503</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>9838.978000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>281984899</v>
       </c>
@@ -1758,8 +1946,16 @@
       <c r="J23">
         <v>14506.29</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>112.2795244508429</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>14377.092000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>282769220</v>
       </c>
@@ -1788,8 +1984,16 @@
       <c r="J24">
         <v>5781.82</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>38.343015544591225</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>5631.0279999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>290486511</v>
       </c>
@@ -1821,8 +2025,16 @@
       <c r="J25">
         <v>12681.34</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>4.3454605016077883</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>9763.0439999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>320623904</v>
       </c>
@@ -1854,8 +2066,16 @@
       <c r="J26">
         <v>10932.55</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>3.5810846222886084</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>7879.69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>432783339</v>
       </c>
@@ -1887,8 +2107,16 @@
       <c r="J27">
         <v>9730.9599999999991</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>63.572791177777184</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>9577.8919999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>446778586</v>
       </c>
@@ -1920,8 +2148,16 @@
       <c r="J28">
         <v>11465.58</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>12.059612386956713</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>10514.838</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>446778587</v>
       </c>
@@ -1949,6 +2185,14 @@
       </c>
       <c r="J29">
         <v>11721.39</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>13.419093150891941</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>10847.903999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>